<commit_message>
Carro e moto finalizados mas temos problemas na coab
</commit_message>
<xml_diff>
--- a/Coisas do junio.xlsx
+++ b/Coisas do junio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusss\locaSpring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3CDC4-1F59-45DD-82E2-E9613230DB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFCDA28-3CEB-40C3-8870-964118BB7D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -356,7 +356,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -425,7 +425,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -467,7 +467,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Caminhonete 100% atualizada bomba patch
</commit_message>
<xml_diff>
--- a/Coisas do junio.xlsx
+++ b/Coisas do junio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusss\locaSpring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFCDA28-3CEB-40C3-8870-964118BB7D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B73B1-A422-4B97-BB3B-2CE25E050C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>LISTA CRUD</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>GUSTAVO</t>
-  </si>
-  <si>
-    <t>Caminhao</t>
   </si>
   <si>
     <t>Caminhonete</t>
@@ -82,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +97,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -138,6 +143,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,7 +364,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -392,7 +400,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -403,7 +411,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -413,8 +421,8 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
+      <c r="B5" s="7">
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>2</v>
@@ -425,41 +433,41 @@
         <v>5</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
-        <v>0.9</v>
+      <c r="B9" s="3">
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -467,10 +475,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -480,9 +488,7 @@
       <c r="B11" s="3">
         <v>0</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -509,7 +515,9 @@
       <c r="B14" s="3">
         <v>0</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -519,20 +527,10 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1518,6 +1516,6 @@
     <mergeCell ref="A1:C2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Cliente and Terceirizado
finalizado CRUD de cliente e terceirizado
</commit_message>
<xml_diff>
--- a/Coisas do junio.xlsx
+++ b/Coisas do junio.xlsx
@@ -119,10 +119,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -366,7 +366,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -377,7 +377,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -388,7 +388,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
@@ -398,7 +398,7 @@
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>0.8</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -410,7 +410,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>0.0</v>
+        <v>0.9</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -420,7 +420,7 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>0.0</v>
       </c>
       <c r="C8" s="3"/>
@@ -429,7 +429,7 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>0.9</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -441,7 +441,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>2</v>
@@ -451,7 +451,7 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1.0</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -462,7 +462,7 @@
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>0.0</v>
       </c>
       <c r="C12" s="3"/>
@@ -471,7 +471,7 @@
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5">
         <v>0.0</v>
       </c>
       <c r="C13" s="3"/>
@@ -480,7 +480,7 @@
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>0.0</v>
       </c>
       <c r="C14" s="3"/>
@@ -490,7 +490,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="4">
-        <v>0.0</v>
+        <v>0.9</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
@@ -500,7 +500,7 @@
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>0.9</v>
       </c>
       <c r="C16" s="3" t="s">

</xml_diff>

<commit_message>
atualizando lista de a fazeres
atualizada
</commit_message>
<xml_diff>
--- a/Coisas do junio.xlsx
+++ b/Coisas do junio.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhYR2RJxJWrpSiuEVn+adCKfcDtxg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgsVyLqAYsvNHxsXlw0ldMi+aYzQQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -431,8 +431,8 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
-        <v>0.9</v>
+      <c r="B9" s="5">
+        <v>1.0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>7</v>
@@ -464,7 +464,7 @@
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>0.95</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -475,7 +475,7 @@
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>1.0</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -497,7 +497,7 @@
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>1.0</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -508,7 +508,7 @@
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>1.0</v>
       </c>
       <c r="C16" s="3" t="s">

</xml_diff>